<commit_message>
added test data for ValidLogin TC
</commit_message>
<xml_diff>
--- a/testdata/input.xlsx
+++ b/testdata/input.xlsx
@@ -1,24 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>HomePageTitle</t>
+  </si>
+  <si>
+    <t>actiTIME - Enter Time-Track</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,13 +374,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -356,7 +417,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>